<commit_message>
starts building the html report
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve">concepto</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">30_05_2023</t>
+    <t xml:space="preserve">21_07_2023</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -56,6 +56,30 @@
   </si>
   <si>
     <t xml:space="preserve">Parrafo. Punto y aparte usando Ctrl+Enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primera oracion de la conclusion final
+Seguna oracion de la conclusion final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduccion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer Renglon de la intro
+Segundo Renglon de la intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objetivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unica oracion del objetivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metodologia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer rengon de los objetivos
+Segundo renglon de los objetivos</t>
   </si>
 </sst>
 </file>
@@ -180,10 +204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,12 +261,48 @@
         <v>36946123</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="243.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="220.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iterates the report adding plots
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -72,14 +72,14 @@
     <t xml:space="preserve">Objetivo</t>
   </si>
   <si>
-    <t xml:space="preserve">Unica oracion del objetivo</t>
+    <t xml:space="preserve">Escalar 7b en la próxima temporada sin lesiones ni molestias</t>
   </si>
   <si>
     <t xml:space="preserve">Metodologia</t>
   </si>
   <si>
-    <t xml:space="preserve">Primer rengon de los objetivos
-Segundo renglon de los objetivos</t>
+    <t xml:space="preserve">Primer rengon de la metodologia
+Segundo renglon de la metodologia</t>
   </si>
 </sst>
 </file>
@@ -206,14 +206,14 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="88.97"/>
   </cols>
   <sheetData>
@@ -261,7 +261,7 @@
         <v>36946123</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="220.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
update to use the new tindeq's cfd feature
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">21_07_2023</t>
+    <t xml:space="preserve">21_09_2023</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -206,7 +206,7 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modifies pullups and beautifies the report
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">21_09_2023</t>
+    <t xml:space="preserve">29_09_2023</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -65,8 +65,13 @@
     <t xml:space="preserve">Introduccion</t>
   </si>
   <si>
-    <t xml:space="preserve">Primer Renglon de la intro
-Segundo Renglon de la intro</t>
+    <t xml:space="preserve">Evaluación de indicadores clave para el rendimiento en la escalada.
+Todas las evaluaciones de dedos son realizadas en una regleta de 20mm de profundidad con un radio de 10 mm
+Fuerza máxima de dedos corresponde a la fuerza que es posible hacer luego de 5 segundo de fuerza isometrica maxima
+Fuerza crítica es la fuerza que se puede ejercer despues de 4 minutos de 7 segundos de esfuerzo máximo y 3 segundos de descanso. Representa la fuerza petado
+La potencia representa la fuerza que se puede ejercer por unidad de segundo. La usamos cuando caemos en una toma en movimiento dinámico y debemos ejercer mucha fuerza en poco tiempo
+Todos los resultados se informan en % del peso corporal ya que así correlacionan mejor con el grado en la biografía
+Comparamos los valores del deportista con referencias poblacionales para comparar con sus pares. Si los indicadores se encuentran por debajo de los valores de referencia, una posibilidad es entrenar para poder desarrollar y mantener mejores valores.</t>
   </si>
   <si>
     <t xml:space="preserve">Objetivo</t>
@@ -78,8 +83,7 @@
     <t xml:space="preserve">Metodologia</t>
   </si>
   <si>
-    <t xml:space="preserve">Primer rengon de la metodologia
-Segundo renglon de la metodologia</t>
+    <t xml:space="preserve">Medición con Tindeq de los indicadores clave informando el grado de escalada según escala IRCRA</t>
   </si>
 </sst>
 </file>
@@ -206,15 +210,15 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="88.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="148.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,7 +276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="132.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -283,7 +287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
@@ -294,7 +298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Corrections after testing usage with another climber and different protocols
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">DD_MM_AAAA</t>
   </si>
   <si>
-    <t xml:space="preserve">20_05_2023</t>
+    <t xml:space="preserve">31_10_2023</t>
   </si>
   <si>
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">29_09_2023</t>
+    <t xml:space="preserve">02_11_2023</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Objetivo</t>
   </si>
   <si>
-    <t xml:space="preserve">Escalar 7b en la próxima temporada sin lesiones ni molestias</t>
+    <t xml:space="preserve">Escalar 7b en la próxima temporada sin lesiones ni molestias y ser feliz</t>
   </si>
   <si>
     <t xml:space="preserve">Metodologia</t>
@@ -210,8 +210,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -262,7 +262,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>36946123</v>
+        <v>37504394</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updates the rfd methodology
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">DD_MM_AAAA</t>
   </si>
   <si>
-    <t xml:space="preserve">31_10_2023</t>
+    <t xml:space="preserve">07_11_2023</t>
   </si>
   <si>
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">02_11_2023</t>
+    <t xml:space="preserve">08_11_2023</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -65,19 +65,47 @@
     <t xml:space="preserve">Introduccion</t>
   </si>
   <si>
-    <t xml:space="preserve">Evaluación de indicadores clave para el rendimiento en la escalada.
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Evaluación de indicadores clave para el rendimiento en la escalada.
 Todas las evaluaciones de dedos son realizadas en una regleta de 20mm de profundidad con un radio de 10 mm
-Fuerza máxima de dedos corresponde a la fuerza que es posible hacer luego de 5 segundo de fuerza isometrica maxima
-Fuerza crítica es la fuerza que se puede ejercer despues de 4 minutos de 7 segundos de esfuerzo máximo y 3 segundos de descanso. Representa la fuerza petado
-La potencia representa la fuerza que se puede ejercer por unidad de segundo. La usamos cuando caemos en una toma en movimiento dinámico y debemos ejercer mucha fuerza en poco tiempo
-Todos los resultados se informan en % del peso corporal ya que así correlacionan mejor con el grado en la biografía
+Fuerza máxima de dedos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(flex-dedo)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> corresponde a la fuerza que es posible hacer luego de 5 segundos de fuerza isometrica maxima
+Fuerza crítica (cfd) es la fuerza que se puede ejercer despues de 4 minutos de 7 segundos de esfuerzo máximo y 3 segundos de descanso. Representa la fuerza petado
+La potencia (rfd) representa la fuerza que se puede ejercer por unidad de segundo. La usamos cuando caemos en una toma en movimiento dinámico y debemos ejercer mucha fuerza en poco tiempo
+Todos los resultados se informan en % del peso corporal ya que así correlacionan mejor con el grado en la bibliografía
 Comparamos los valores del deportista con referencias poblacionales para comparar con sus pares. Si los indicadores se encuentran por debajo de los valores de referencia, una posibilidad es entrenar para poder desarrollar y mantener mejores valores.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Objetivo</t>
   </si>
   <si>
-    <t xml:space="preserve">Escalar 7b en la próxima temporada sin lesiones ni molestias y ser feliz</t>
+    <t xml:space="preserve">Escalar 8a en la próxima temporada sin lesiones ni molestias y ser feliz</t>
   </si>
   <si>
     <t xml:space="preserve">Metodologia</t>
@@ -93,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -123,6 +151,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,8 +244,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,15 +288,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>37504394</v>
+      <c r="C4" s="3" t="n">
+        <v>41089526</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
corrige la app para ajustarse a las modificaciones de la app de tindeq
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">DD_MM_AAAA</t>
   </si>
   <si>
-    <t xml:space="preserve">07_11_2023</t>
+    <t xml:space="preserve">12_01_2025</t>
   </si>
   <si>
     <t xml:space="preserve">fecha2</t>
   </si>
   <si>
-    <t xml:space="preserve">08_11_2023</t>
+    <t xml:space="preserve">14_01_2025</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -65,47 +65,19 @@
     <t xml:space="preserve">Introduccion</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Evaluación de indicadores clave para el rendimiento en la escalada.
+    <t xml:space="preserve">Evaluación de indicadores clave para el rendimiento en la escalada.
 Todas las evaluaciones de dedos son realizadas en una regleta de 20mm de profundidad con un radio de 10 mm
-Fuerza máxima de dedos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(flex-dedo)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> corresponde a la fuerza que es posible hacer luego de 5 segundos de fuerza isometrica maxima
+Fuerza máxima de dedos (flex-dedo) corresponde a la fuerza que es posible hacer luego de 5 segundos de fuerza isometrica maxima
 Fuerza crítica (cfd) es la fuerza que se puede ejercer despues de 4 minutos de 7 segundos de esfuerzo máximo y 3 segundos de descanso. Representa la fuerza petado
 La potencia (rfd) representa la fuerza que se puede ejercer por unidad de segundo. La usamos cuando caemos en una toma en movimiento dinámico y debemos ejercer mucha fuerza en poco tiempo
 Todos los resultados se informan en % del peso corporal ya que así correlacionan mejor con el grado en la bibliografía
 Comparamos los valores del deportista con referencias poblacionales para comparar con sus pares. Si los indicadores se encuentran por debajo de los valores de referencia, una posibilidad es entrenar para poder desarrollar y mantener mejores valores.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Objetivo</t>
   </si>
   <si>
-    <t xml:space="preserve">Escalar 8a en la próxima temporada sin lesiones ni molestias y ser feliz</t>
+    <t xml:space="preserve">Escalar 8a en la próxima temporada sin lesiones ni molestias</t>
   </si>
   <si>
     <t xml:space="preserve">Metodologia</t>
@@ -121,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -151,12 +123,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,7 +210,7 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -252,7 +218,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="148.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +250,7 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -296,10 +262,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>41089526</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>30282627</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
@@ -310,7 +276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="132.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="165.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
cambio para evaluar en una sola fecha y que se pueda actualizar todo el dataset de una
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t xml:space="preserve">concepto</t>
   </si>
@@ -31,19 +31,13 @@
     <t xml:space="preserve">valor</t>
   </si>
   <si>
-    <t xml:space="preserve">fecha1</t>
+    <t xml:space="preserve">fecha</t>
   </si>
   <si>
     <t xml:space="preserve">DD_MM_AAAA</t>
   </si>
   <si>
-    <t xml:space="preserve">12_01_2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecha2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14_01_2025</t>
+    <t xml:space="preserve">29_01_2025</t>
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
@@ -77,7 +71,7 @@
     <t xml:space="preserve">Objetivo</t>
   </si>
   <si>
-    <t xml:space="preserve">Escalar 8a en la próxima temporada sin lesiones ni molestias</t>
+    <t xml:space="preserve">Escalar 8b+ en marzo comodo</t>
   </si>
   <si>
     <t xml:space="preserve">Metodologia</t>
@@ -208,10 +202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -247,68 +241,58 @@
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="3" t="n">
+        <v>34483112</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <v>30282627</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="165.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="165.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>